<commit_message>
:bug: all entries from excel file are populated
</commit_message>
<xml_diff>
--- a/Test/exemplo lista.xlsx
+++ b/Test/exemplo lista.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I557579\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\ruthiel\projects\sanctions-engine\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF0D986-DFBA-462F-8F6B-B450A3820671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFFF2F5-0E4F-4543-8220-AA74102C9DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="38700" windowHeight="15105" xr2:uid="{EBD16A9E-5AED-2B4C-B992-E97E504B8E31}"/>
+    <workbookView xWindow="5370" yWindow="5370" windowWidth="38700" windowHeight="15105" xr2:uid="{EBD16A9E-5AED-2B4C-B992-E97E504B8E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Apple Inc</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Emitente</t>
+  </si>
+  <si>
+    <t>Apple Limitada</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -421,7 +424,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
:sparkles: URL configuration working
</commit_message>
<xml_diff>
--- a/Test/exemplo lista.xlsx
+++ b/Test/exemplo lista.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\ruthiel\projects\sanctions-engine\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974D2FCC-2868-4E74-9763-848D40D6F11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0108A185-EB49-4D1B-B1FB-6B85EA2ED019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="5715" windowWidth="38700" windowHeight="15105" xr2:uid="{EBD16A9E-5AED-2B4C-B992-E97E504B8E31}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="10920" xr2:uid="{EBD16A9E-5AED-2B4C-B992-E97E504B8E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Apple Inc</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Apple Limitada</t>
+  </si>
+  <si>
+    <t>ROSHAN Money EXCHANGE</t>
   </si>
   <si>
     <t>ROSHAN MONEY EXCHANGE</t>
@@ -406,7 +409,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -450,6 +453,9 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>